<commit_message>
test data & eval script updated
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Presidio\presidio\presidio\FunctionAPPCiCd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B2158A-C4A7-45C8-A966-BB2750321BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3785804-9DD1-412C-9EED-06965A2D64CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{553DE523-E820-42A8-B4FD-6D57A57A9D54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>Input Data</t>
   </si>
@@ -119,24 +119,6 @@
     <t>Scenario Prompt</t>
   </si>
   <si>
-    <t>You are a data validation assistant to validate the actual result against the ground truth.
-    Given the following JSON data:
-    - Extracted Value: {extracted_value}
-    - Expense Details: {details_value}
-    - Ground Truth: {ground_truth}
-    - Reconciled Data Section: {reconciled_data}
-    Validate whether the employee name from Extracted Value matches with relevant field from Expense Details.
-    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
-    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
-    If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
-    Otherwise, respond with "Fail".
-    Return your response strictly in the following JSON format:
-    {{
-    "Result": "Pass or Fail",
-    "Reason": "Reason for failure or how we can conclude it as Pass"
-    }}</t>
-  </si>
-  <si>
     <t>{"expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","extracted_data":{"employee_name":"Barbara Siminerio","employee_name_metadata":{"x":0.6747,"y":2.444,"width":0.9527,"height":0.123,"page_no":1},"vendor_name":"Courtyard by Marriott® New York Manhattan Midtown West","vendor_name_metadata":{"x":0.493,"y":1.1993,"width":3.172,"height":0.1332,"page_no":1},"transaction_date":"05Sep25","transaction_date_metadata":{"x":5.1738,"y":3.3066,"width":0.807,"height":0.1221,"page_no":1},"checkin_date":"02Sep25","checkin_date_metadata":{"x":0.6719,"y":3.3056,"width":0.858,"height":0.1314,"page_no":1},"checkout_date":"05Sep25","checkout_date_metadata":{"x":3.6722,"y":3.3058,"width":0.9043,"height":0.1362,"page_no":1},"transaction_amount":1487.31,"transaction_amount_metadata":{"x":7.1581,"y":6.2522,"width":0.4173,"height":0.1208,"page_no":1},"currency":"$","currency_metadata":{"x":5.1748,"y":2.9762,"width":0.7483,"height":0.1211,"page_no":1},"attendee_count":1,"attendee_count_metadata":{"x":5.1739,"y":2.798,"width":1.088,"height":0.1229,"page_no":1},"payment_mode":"American Express","payment_mode_metadata":{"x":1.7402,"y":6.2557,"width":0.9722,"height":0.13,"page_no":1},"availability_exceptionapproval":true,"approvers_mailid":"CFOTravelException@cognizant.com","items":[{"date":"02Sep25","amount":490.77},{"date":"03Sep25","amount":490.77},{"date":"04Sep25","amount":490.77}]},"expense_details":{"id":"22543708-dd61-434a-9946-514b02d74afa","report_id":"37F7BC25E9F943EFA87D","download_date":"07-10-2025","expense_id":"7635BF521DB19E419E9DE80A659214C7","emp_id":"127957","emp_name":"Barbara Siminerio","pta_code":"127957-F78F9_BOM-BLR 09/07/2022","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","receipt_ImageId":"1E9B3040BAA04FF987006144FDF4C771","receipt_available":true,"exp_receipt_filename":"37F7BC25E9F943EFA87D/7635BF521DB19E419E9DE80A659214C7/Hotel/1E9B3040BAA04FF987006144FDF4C771.pdf","transaction_amount":1487.31,"currency":"USD","transaction_date":"2025-09-04","personal_expense":false,"bill_to_client":false,"expense_rejected":false,"vendor_name":"CY NY MIDTOWN WEST","business_purpose":"Q3 2025 Board Meeting - BS","attendee_count":0,"mileage":null,"itemization_details":[{"expense_id":"E31AF0F8BC44A843A207366C4C52E990","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":429,"currency":"USD","transaction_date":"2025-09-02","personal_expense":false,"attendee_count":0},{"expense_id":"57517C154BD15348AB58DADEC09237DF","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel Tax","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":66.77,"currency":"USD","transaction_date":"2025-09-02","personal_expense":false,"attendee_count":0},{"expense_id":"0FB3669F532FE045B79D79B71ADFD2D5","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":429,"currency":"USD","transaction_date":"2025-09-03","personal_expense":false,"attendee_count":0},{"expense_id":"627429F89645124DB88AD7EF24A0952B","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel Tax","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":66.77,"currency":"USD","transaction_date":"2025-09-03","personal_expense":false,"attendee_count":0},{"expense_id":"7E87C51C4BBA1C4EA0876B2EAB656F57","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":429,"currency":"USD","transaction_date":"2025-09-04","personal_expense":false,"attendee_count":0},{"expense_id":"3BD65773F4268C479523C83D07223BEE","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel Tax","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":66.77,"currency":"USD","transaction_date":"2025-09-04","personal_expense":false,"attendee_count":0}],"attendee_details":[],"trip_details":[],"comments":[],"status":"Pending","_rid":"O9gqANpzYzkoAAAAAAAAAA==","_self":"dbs/O9gqAA==/colls/O9gqANpzYzk=/docs/O9gqANpzYzkoAAAAAAAAAA==/","_etag":"\"38015d28-0000-0100-0000-68e4f41d0000\"","_attachments":"attachments/","_ts":1759835165}}</t>
   </si>
   <si>
@@ -161,24 +143,6 @@
       }</t>
   </si>
   <si>
-    <t>You are a data validation assistant to validate the actual result against the ground truth.
-    Given the following JSON data:
-    - Extracted Value: {extracted_value}
-    - Expense Details: {details_value}
-    - Ground Truth: {ground_truth}
-    - Reconciled Data Section: {reconciled_data}
-    Validate whether the transaction amount from Extracted Value matches with relevant field from Expense Details.
-    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
-    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
-    If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
-    Otherwise, respond with "Fail".
-    Return your response strictly in the following JSON format:
-    {{
-    "Result": "Pass or Fail",
-    "Reason": "Reason for failure or how we can conclude it as Pass"
-    }}</t>
-  </si>
-  <si>
     <t>{
         "field_name": "transaction_amount",
         "receipt_value": "1487.31",
@@ -188,25 +152,6 @@
       }</t>
   </si>
   <si>
-    <t>You are a data validation assistant to validate the actual result against the ground truth.
-    Given the following JSON data:
-    - Extracted Value: {extracted_value}
-    - Expense Details: {details_value}
-    - Ground Truth: {ground_truth}
-    - Reconciled Data Section: {reconciled_data}
-    Validate whether the vendor name from Extracted Value matches with relevant field from Expense Details.
-    Please note that different names or abbreviations may refer to the same hotel or location. If you encounter multiple names for a property, they are likely interchangeable	
-    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
-    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
-    If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
-    Otherwise, respond with "Fail".
-    Return your response strictly in the following JSON format:
-    {{
-    "Result": "Pass or Fail",
-    "Reason": "Reason for failure or how we can conclude it as Pass"
-    }}</t>
-  </si>
-  <si>
     <t>{"expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","extracted_data":{"employee_name":"Barbara Siminerio","employee_name_metadata":{"x":0.6747,"y":2.444,"width":0.9527,"height":0.123,"page_no":1},"vendor_name":"Courtyard by Marriott® New York Manhattan Midtown West","vendor_name_metadata":{"x":0.493,"y":1.1993,"width":3.172,"height":0.1332,"page_no":1},"transaction_date":"05Sep25","transaction_date_metadata":{"x":5.1738,"y":3.3066,"width":0.807,"height":0.1221,"page_no":1},"checkin_date":"02Sep25","checkin_date_metadata":{"x":0.6719,"y":3.3056,"width":0.858,"height":0.1314,"page_no":1},"checkout_date":"05Sep25","checkout_date_metadata":{"x":3.6722,"y":3.3058,"width":0.9043,"height":0.1362,"page_no":1},"transaction_amount":1487.31,"transaction_amount_metadata":{"x":7.1581,"y":6.2522,"width":0.4173,"height":0.1208,"page_no":1},"currency":"$","currency_metadata":{"x":5.1748,"y":2.9762,"width":0.7483,"height":0.1211,"page_no":1},"attendee_count":1,"attendee_count_metadata":{"x":5.1739,"y":2.798,"width":1.088,"height":0.1229,"page_no":1},"payment_mode":"American Express","payment_mode_metadata":{"x":1.7402,"y":6.2557,"width":0.9722,"height":0.13,"page_no":1},"availability_exceptionapproval":true,"approvers_mailid":"CFOTravelException@cognizant.com","items":[{"date":"02Sep25","amount":490.77},{"date":"03Sep25","amount":490.77},{"date":"04Sep25","amount":490.77}]},"expense_details":{"id":"22543708-dd61-434a-9946-514b02d74afa","report_id":"37F7BC25E9F943EFA87D","download_date":"07-10-2025","expense_id":"7635BF521DB19E419E9DE80A659214C7","emp_id":"127957","emp_name":"Eswarachari Vasant","pta_code":"127957-F78F9_BOM-BLR 09/07/2022","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","receipt_ImageId":"1E9B3040BAA04FF987006144FDF4C771","receipt_available":true,"exp_receipt_filename":"37F7BC25E9F943EFA87D/7635BF521DB19E419E9DE80A659214C7/Hotel/1E9B3040BAA04FF987006144FDF4C771.pdf","transaction_amount":1497.31,"currency":"USD","transaction_date":"2025-09-04","personal_expense":false,"bill_to_client":false,"expense_rejected":false,"vendor_name":"HILTON NY MIDTOWN WEST","business_purpose":"Q3 2025 Board Meeting - BS","attendee_count":0,"mileage":null,"itemization_details":[{"expense_id":"E31AF0F8BC44A843A207366C4C52E990","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":429,"currency":"USD","transaction_date":"2025-09-02","personal_expense":false,"attendee_count":0},{"expense_id":"57517C154BD15348AB58DADEC09237DF","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel Tax","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":66.77,"currency":"USD","transaction_date":"2025-09-02","personal_expense":false,"attendee_count":0},{"expense_id":"0FB3669F532FE045B79D79B71ADFD2D5","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":429,"currency":"USD","transaction_date":"2025-09-03","personal_expense":false,"attendee_count":0},{"expense_id":"627429F89645124DB88AD7EF24A0952B","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel Tax","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":66.77,"currency":"USD","transaction_date":"2025-09-03","personal_expense":false,"attendee_count":0},{"expense_id":"7E87C51C4BBA1C4EA0876B2EAB656F57","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":429,"currency":"USD","transaction_date":"2025-09-04","personal_expense":false,"attendee_count":0},{"expense_id":"3BD65773F4268C479523C83D07223BEE","parent_expense_id":"7635BF521DB19E419E9DE80A659214C7","expense_type":"Hotel Tax","location":"New York, New York","payment_type":"Cash/Out-of-Pocket","transaction_amount":66.77,"currency":"USD","transaction_date":"2025-09-04","personal_expense":false,"attendee_count":0}],"attendee_details":[],"trip_details":[],"comments":[],"status":"Pending","_rid":"O9gqANpzYzkoAAAAAAAAAA==","_self":"dbs/O9gqAA==/colls/O9gqANpzYzk=/docs/O9gqANpzYzkoAAAAAAAAAA==/","_etag":"\"38015d28-0000-0100-0000-68e4f41d0000\"","_attachments":"attachments/","_ts":1759835165}}</t>
   </si>
   <si>
@@ -228,25 +173,6 @@
       }</t>
   </si>
   <si>
-    <t>You are a data validation assistant to validate the actual result against the ground truth.
-    Given the following JSON data:
-    - Extracted Value: {extracted_value}
-    - Expense Details: {details_value}
-    - Ground Truth: {ground_truth}
-    - Reconciled Data Section: {reconciled_data}
-    Validate whether the transaction date from Extracted Value matches with relevant field from Expense Details.
-    Transaction date might be same between Expense Details and Extracted Value or vary by 1 or 2 days
-    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
-    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
-    If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
-    Otherwise, respond with "Fail".
-    Return your response strictly in the following JSON format:
-    {{
-    "Result": "Pass or Fail",
-    "Reason": "Reason for failure or how we can conclude it as Pass"
-    }}</t>
-  </si>
-  <si>
     <t>{
         "field_name": "transaction_date",
         "receipt_value": "05-09-2025",
@@ -268,24 +194,6 @@
       }</t>
   </si>
   <si>
-    <t>You are a data validation assistant to validate the actual result against the ground truth.
-    Given the following JSON data:
-    - Extracted Value: {extracted_value}
-    - Expense Details: {details_value}
-    - Ground Truth: {ground_truth}
-    - Reconciled Data Section: {reconciled_data}
-    Validate whether the currency from Extracted Value matches with relevant field from Expense Details.
-    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
-    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
-    If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
-    Otherwise, respond with "Fail".
-    Return your response strictly in the following JSON format:
-    {{
-    "Result": "Pass or Fail",
-    "Reason": "Reason for failure or how we can conclude it as Pass"
-    }}</t>
-  </si>
-  <si>
     <t>{
         "field_name": "currency",
         "receipt_value": "$",
@@ -305,26 +213,6 @@
         "match": "false",
         "details": "Currency symbols are not matching"
       }</t>
-  </si>
-  <si>
-    <t>You are a data validation assistant to validate the actual result against the ground truth.
-    Given the following JSON data:
-    - Extracted Value: {extracted_value}
-    - Expense Details: {details_value}
-    - Ground Truth: {ground_truth}
-    - Reconciled Data Section: {reconciled_data}
-    Validate whether the vendor name from Extracted Value matches with relevant field from Expense Details.
-    Please note that different names or abbreviations may refer to the same hotel or location. If you encounter multiple names for a property, they are likely interchangeable	
-    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
-    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
-    Please check the relevant meaning of the reason. Don't expect the reason is always same and consistent     
-    If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
-    Otherwise, respond with "Fail".
-    Return your response strictly in the following JSON format:
-    {{
-    "Result": "Pass or Fail",
-    "Reason": "Reason for failure or how we can conclude it as Pass"
-    }}</t>
   </si>
   <si>
     <t xml:space="preserve">Payment mode :match between concur &amp; CWT receipt or Itinerary </t>
@@ -349,12 +237,167 @@
     "Reason": "Reason for failure or how we can conclude it as Pass"
     }}</t>
   </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the employee name from Extracted Value matches with relevant field from Expense Details.
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+  **IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the employee name from Extracted Value matches with relevant field from Expense Details.
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+**IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the transaction amount from Extracted Value matches with relevant field from Expense Details.
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+**IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the transaction amount from Extracted Value matches with relevant field from Expense Details.
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+  **IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the vendor name from Extracted Value matches with relevant field from Expense Details.
+    Please note that different names or abbreviations may refer to the same hotel or location. If you encounter multiple names for a property, they are likely interchangeable	
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+**IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the vendor name from Extracted Value matches with relevant field from Expense Details.
+    Please note that different names or abbreviations may refer to the same hotel or location. If you encounter multiple names for a property, they are likely interchangeable	
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+    Please check the relevant meaning of the reason. Don't expect the reason is always same and consistent     
+**IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the currency from Extracted Value matches with relevant field from Expense Details.
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+**IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
+  <si>
+    <t>You are a data validation assistant to validate the actual result against the ground truth.
+    Given the following JSON data:
+    - Extracted Value: {extracted_value}
+    - Expense Details: {details_value}
+    - Ground Truth: {ground_truth}
+    - Reconciled Data Section: {reconciled_data}
+    Validate whether the currency from Extracted Value matches with relevant field from Expense Details.
+    If it is matched or not matched, verify that this match is accurately reflected in the Ground Truth JSON, specifically in the Reconciled Data section.
+    Additionally, confirm whether both the data and failure reason are captured in the Reconciled Data section.
+**IMPORTANT**
+	Though there are mismatches, If the result is captured in the reconciled data and the ground truth, respond with "Pass" in the Result.
+    Otherwise, respond with "Fail".
+    Return your response strictly in the following JSON format:
+    {{
+    "Result": "Pass or Fail",
+    "Reason": "Reason for failure or how we can conclude it as Pass"
+    }}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,16 +412,23 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="3"/>
+      <sz val="1"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="1"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -422,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,12 +484,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,17 +827,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538F2F68-B832-4B8A-8090-95FB615BD679}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
     <col min="3" max="3" width="12.90625" customWidth="1"/>
-    <col min="4" max="4" width="59" customWidth="1"/>
-    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" customWidth="1"/>
+    <col min="5" max="5" width="40" style="7" customWidth="1"/>
     <col min="6" max="6" width="19.7265625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="16.453125" customWidth="1"/>
@@ -806,7 +857,7 @@
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -822,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="291.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -833,23 +884,23 @@
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>25</v>
+      <c r="E2" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>26</v>
+      <c r="G2" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="291.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -860,13 +911,13 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>25</v>
+      <c r="E3" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -876,7 +927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -884,10 +935,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
@@ -895,7 +946,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -903,10 +954,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
@@ -914,7 +965,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="291.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -925,23 +976,23 @@
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>30</v>
+      <c r="E6" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="291.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -952,23 +1003,23 @@
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
+      <c r="E7" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>28</v>
+      <c r="G7" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="321.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -979,23 +1030,23 @@
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>32</v>
+      <c r="E8" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>28</v>
+      <c r="G8" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="341.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1006,23 +1057,23 @@
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>44</v>
+      <c r="E9" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>33</v>
+      <c r="G9" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="311.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1033,23 +1084,23 @@
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>36</v>
+      <c r="E10" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>28</v>
+      <c r="G10" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="311.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1060,23 +1111,23 @@
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>46</v>
+      <c r="E11" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>38</v>
+      <c r="G11" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="301.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1087,23 +1138,23 @@
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>40</v>
+      <c r="E12" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>38</v>
+      <c r="G12" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="166.5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="311.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1114,20 +1165,20 @@
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>40</v>
+      <c r="E13" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>42</v>
+      <c r="G13" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>